<commit_message>
iOS app icon, nav.js, Anforderungen.xlsx
</commit_message>
<xml_diff>
--- a/Doc/Anforderungen.xlsx
+++ b/Doc/Anforderungen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Antwort-Zeiten, Usability, Sicherheit, verwendete Technologie.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Beim Beantworten dauert die Anzeige ob richtig oder falsch maximal eine Sekunde.</t>
   </si>
@@ -39,6 +36,39 @@
   </si>
   <si>
     <t>MySQL</t>
+  </si>
+  <si>
+    <t>Der User kann sein Konto löschen. (Sicherheit)</t>
+  </si>
+  <si>
+    <t>jQuery</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>Verwendete Technologien:</t>
+  </si>
+  <si>
+    <t>(SpotifyAPI)</t>
+  </si>
+  <si>
+    <t>Antwortzeiten</t>
+  </si>
+  <si>
+    <t>Sicherheit</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Das Game benötigt keine Anleitung.</t>
+  </si>
+  <si>
+    <t>Nicht funktionale Anforderungen an SongQuiz</t>
   </si>
 </sst>
 </file>
@@ -353,43 +383,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="94.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>3</v>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>